<commit_message>
commiting data models for credit, student, Degree
</commit_message>
<xml_diff>
--- a/dotnet.xlsx
+++ b/dotnet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="4545" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="107">
   <si>
     <t>PK: CreditID</t>
   </si>
@@ -207,12 +207,6 @@
     <t>PK: StudentID</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Given</t>
-  </si>
-  <si>
     <t>SID</t>
   </si>
   <si>
@@ -343,6 +337,15 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>CatPawsID</t>
+  </si>
+  <si>
+    <t>GivenName</t>
+  </si>
+  <si>
+    <t>FamilyName</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -758,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1">
@@ -5724,8 +5727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5743,16 +5746,16 @@
         <v>59</v>
       </c>
       <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1">
-        <v>919</v>
+      <c r="E1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1">
@@ -5760,13 +5763,13 @@
         <v>533619</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="E2" s="8">
         <v>919568817</v>
@@ -5777,13 +5780,13 @@
         <v>533907</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="E3" s="7">
         <v>919570703</v>
@@ -5794,13 +5797,13 @@
         <v>533623</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="E4" s="5">
         <v>919568816</v>
@@ -7061,7 +7064,7 @@
         <v>460</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1">
@@ -7078,7 +7081,7 @@
         <v>356</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1">
@@ -7095,7 +7098,7 @@
         <v>542</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1">
@@ -7112,7 +7115,7 @@
         <v>563</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1">
@@ -7282,7 +7285,7 @@
         <v>356</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7299,7 +7302,7 @@
         <v>542</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7316,7 +7319,7 @@
         <v>563</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7333,7 +7336,7 @@
         <v>460</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7350,7 +7353,7 @@
         <v>560</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7367,7 +7370,7 @@
         <v>664</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7384,7 +7387,7 @@
         <v>64</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7503,7 +7506,7 @@
         <v>460</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7520,7 +7523,7 @@
         <v>356</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7537,7 +7540,7 @@
         <v>542</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7554,7 +7557,7 @@
         <v>563</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7571,7 +7574,7 @@
         <v>560</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7588,7 +7591,7 @@
         <v>64</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7605,7 +7608,7 @@
         <v>555</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
@@ -7724,7 +7727,7 @@
         <v>460</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7741,7 +7744,7 @@
         <v>356</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7758,7 +7761,7 @@
         <v>542</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7775,7 +7778,7 @@
         <v>563</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7792,7 +7795,7 @@
         <v>691</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7809,7 +7812,7 @@
         <v>618</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7826,7 +7829,7 @@
         <v>692</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7843,7 +7846,7 @@
         <v>560</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7860,7 +7863,7 @@
         <v>555</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7877,7 +7880,7 @@
         <v>643</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7894,7 +7897,7 @@
         <v>20</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
@@ -7945,7 +7948,7 @@
         <v>460</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
@@ -7962,7 +7965,7 @@
         <v>356</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
@@ -7979,7 +7982,7 @@
         <v>542</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
@@ -9096,19 +9099,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1">
@@ -9122,10 +9125,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1">
@@ -9139,10 +9142,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1">
@@ -9156,10 +9159,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1">
@@ -9173,10 +9176,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1">
@@ -9190,10 +9193,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1">
@@ -9207,10 +9210,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="5" customFormat="1">
@@ -9224,10 +9227,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1">
@@ -9241,10 +9244,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1">
@@ -9258,10 +9261,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1">
@@ -9275,10 +9278,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1">
@@ -9292,10 +9295,10 @@
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="7" customFormat="1">
@@ -9309,10 +9312,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="7" customFormat="1">
@@ -9326,10 +9329,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="7" customFormat="1">
@@ -9343,10 +9346,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="7" customFormat="1">
@@ -9360,10 +9363,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="7" customFormat="1">
@@ -9377,10 +9380,10 @@
         <v>5</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:5">

</xml_diff>

<commit_message>
commiting DbInitializer.cs with Student and DegreePlan data
</commit_message>
<xml_diff>
--- a/dotnet.xlsx
+++ b/dotnet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533619\Documents\44663\Degreeplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533623\Documents\44663\Degreeplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="4545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="4545" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
   <si>
     <t>PK: CreditID</t>
   </si>
@@ -93,9 +93,6 @@
     <t xml:space="preserve">MS ACS </t>
   </si>
   <si>
-    <t>Databases</t>
-  </si>
-  <si>
     <t>NF</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Web apps</t>
   </si>
   <si>
-    <t>Advanced Databses</t>
-  </si>
-  <si>
     <t>664-UX</t>
   </si>
   <si>
@@ -159,12 +153,6 @@
     <t>Elective2</t>
   </si>
   <si>
-    <t>PK: DegreePlanID</t>
-  </si>
-  <si>
-    <t>FK: StudentID</t>
-  </si>
-  <si>
     <t>DegreePlanAbv</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>PK: StudentID</t>
-  </si>
-  <si>
     <t>SID</t>
   </si>
   <si>
@@ -349,6 +334,24 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>DegreeplanID</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Advanced Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> StudentID</t>
+  </si>
+  <si>
+    <t>DegreePlanID</t>
+  </si>
+  <si>
+    <t>StudentID</t>
   </si>
 </sst>
 </file>
@@ -764,7 +767,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1">
@@ -817,7 +820,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="11" t="str">
-        <f t="shared" ref="E3:E5" si="0">" new Degree{"&amp;$A$1&amp;" = "&amp;A4 &amp; " , "&amp;$B$1 &amp; " = '" &amp;B4&amp;"' , "&amp;$C$1&amp;" = '" &amp;C4&amp;"'},"</f>
+        <f t="shared" ref="E4:E5" si="0">" new Degree{"&amp;$A$1&amp;" = "&amp;A4 &amp; " , "&amp;$B$1 &amp; " = '" &amp;B4&amp;"' , "&amp;$C$1&amp;" = '" &amp;C4&amp;"'},"</f>
         <v xml:space="preserve"> new Degree{PK: DegreeID = 3 , DegreeAbv = 'ACS+NF' , DegreeName = 'MS ACS + NF'},</v>
       </c>
     </row>
@@ -1829,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1865,7 +1868,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1876,7 +1879,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1889,7 +1892,7 @@
       </c>
       <c r="G2" t="str">
         <f>" new Credit{"&amp;$A$1&amp;" ="&amp;A2&amp;" , "&amp;$B$1&amp;" ="&amp;B2&amp;" , "&amp;$C$1&amp;" ="&amp;C2&amp;" , "&amp;$D$1&amp;" ="&amp;D2&amp;", "&amp;$E$1&amp;" ="&amp;E2&amp;" , "&amp;$F$1&amp;" , "&amp;F2&amp;"}"</f>
-        <v xml:space="preserve"> new Credit{PK: CreditID =460 , CreditAbv =DB , CreditName =Databases , IsSummer =0, IsSpring =1 , IsFall , 1}</v>
+        <v xml:space="preserve"> new Credit{PK: CreditID =460 , CreditAbv =DB , CreditName =Database , IsSummer =0, IsSpring =1 , IsFall , 1}</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1897,10 +1900,10 @@
         <v>356</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1924,7 +1927,7 @@
         <v>542</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1948,7 +1951,7 @@
         <v>563</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1972,7 +1975,7 @@
         <v>560</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1985,7 +1988,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Credit{PK: CreditID =560 , CreditAbv =560 , CreditName =Advanced Databses , IsSummer =1, IsSpring =1 , IsFall , 1}</v>
+        <v xml:space="preserve"> new Credit{PK: CreditID =560 , CreditAbv =560 , CreditName =Advanced Database , IsSummer =1, IsSpring =1 , IsFall , 1}</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1993,10 +1996,10 @@
         <v>664</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2017,10 +2020,10 @@
         <v>618</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2041,10 +2044,10 @@
         <v>555</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2065,10 +2068,10 @@
         <v>691</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2089,10 +2092,10 @@
         <v>692</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2113,10 +2116,10 @@
         <v>64</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2137,10 +2140,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2161,10 +2164,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3172,7 +3175,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3337,406 +3340,86 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>460</v>
-      </c>
-    </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="1">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="1">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="1">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="1">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="1">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="1">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="1">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1">
-        <v>5</v>
-      </c>
-      <c r="C49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1"/>
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="33" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="35" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="36" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="37" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="38" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="39" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="40" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="41" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="42" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="43" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="44" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="45" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="46" spans="2:3" ht="15.75" customHeight="1"/>
+    <row r="47" spans="2:3" ht="15.75" customHeight="1">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="51" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="52" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="53" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="54" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="55" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="56" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="57" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="58" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="59" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="60" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="61" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="62" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="63" spans="2:2" ht="15.75" customHeight="1"/>
+    <row r="64" spans="2:2" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -4681,10 +4364,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4697,72 +4380,84 @@
     <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1">
       <c r="A2" s="8">
         <v>533619</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" s="8">
         <v>919568817</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="7" customFormat="1">
+      <c r="F2" s="8" t="str">
+        <f>"Student {"&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;B2&amp;", "&amp;$C$1&amp;"="&amp;C2&amp;", "&amp;$D$1&amp;"="&amp;D2&amp;", "&amp;$E$1&amp;"="&amp;E2&amp;"},"</f>
+        <v>Student { StudentID=533619, FamilyName=Cheekoti, GivenName=Vennela, SID=S533619, CatPawsID=919568817},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1">
       <c r="A3" s="7">
         <v>533907</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" s="7">
         <v>919570703</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="5" customFormat="1">
+      <c r="F3" s="8" t="str">
+        <f t="shared" ref="F3:F4" si="0">"Student {"&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;B3&amp;", "&amp;$C$1&amp;"="&amp;C3&amp;", "&amp;$D$1&amp;"="&amp;D3&amp;", "&amp;$E$1&amp;"="&amp;E3&amp;"},"</f>
+        <v>Student { StudentID=533907, FamilyName=Gade, GivenName=Susritha, SID=S533907, CatPawsID=919570703},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5">
         <v>533623</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5">
         <v>919568816</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Student { StudentID=533623, FamilyName=Gone, GivenName=Sathwika, SID=S533623, CatPawsID=919568816},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -5753,10 +5448,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5769,24 +5464,24 @@
     <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1">
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1">
       <c r="A2" s="8">
         <v>7251</v>
       </c>
@@ -5794,16 +5489,20 @@
         <v>533619</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1">
+      <c r="F2" s="8" t="str">
+        <f>"DegreePlan {"&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;B2&amp;", "&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;"},"</f>
+        <v>DegreePlan {DegreePlanID=7251, StudentID=533619, DegreePlanAbv=Super Fast,DegreePlanName=As Fast as I can,FK:DegreeID=1},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1">
       <c r="A3" s="8">
         <v>7258</v>
       </c>
@@ -5811,16 +5510,20 @@
         <v>533619</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="5" customFormat="1">
+      <c r="F3" s="8" t="str">
+        <f>"DegreePlan {"&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;B3&amp;", "&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;"},"</f>
+        <v>DegreePlan {DegreePlanID=7258, StudentID=533619, DegreePlanAbv=slow and Easy,DegreePlanName=As slow as I can,FK:DegreeID=1},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5">
         <v>7253</v>
       </c>
@@ -5828,16 +5531,20 @@
         <v>533623</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="7" customFormat="1">
+      <c r="F4" s="8" t="str">
+        <f>"DegreePlan {"&amp;$A$1&amp;"="&amp;A4&amp;", "&amp;$B$1&amp;"="&amp;B4&amp;", "&amp;$C$1&amp;"="&amp;C4&amp;","&amp;$D$1&amp;"="&amp;D4&amp;","&amp;$E$1&amp;"="&amp;E4&amp;"},"</f>
+        <v>DegreePlan {DegreePlanID=7253, StudentID=533623, DegreePlanAbv=Super Fast,DegreePlanName=As Fast as I can,FK:DegreeID=1},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1">
       <c r="A5" s="7">
         <v>7255</v>
       </c>
@@ -5845,16 +5552,20 @@
         <v>533907</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="7" customFormat="1">
+      <c r="F5" s="8" t="str">
+        <f>"DegreePlan {"&amp;$A$1&amp;"="&amp;A5&amp;", "&amp;$B$1&amp;"="&amp;B5&amp;", "&amp;$C$1&amp;"="&amp;C5&amp;","&amp;$D$1&amp;"="&amp;D5&amp;","&amp;$E$1&amp;"="&amp;E5&amp;"},"</f>
+        <v>DegreePlan {DegreePlanID=7255, StudentID=533907, DegreePlanAbv=Slow and Easy,DegreePlanName=As slow as I can,FK:DegreeID=1},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="7" customFormat="1">
       <c r="A6" s="7">
         <v>7257</v>
       </c>
@@ -5862,16 +5573,20 @@
         <v>533907</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="5" customFormat="1">
+      <c r="F6" s="8" t="str">
+        <f>"DegreePlan {"&amp;$A$1&amp;"="&amp;A6&amp;", "&amp;$B$1&amp;"="&amp;B6&amp;", "&amp;$C$1&amp;"="&amp;C6&amp;","&amp;$D$1&amp;"="&amp;D6&amp;","&amp;$E$1&amp;"="&amp;E6&amp;"},"</f>
+        <v>DegreePlan {DegreePlanID=7257, StudentID=533907, DegreePlanAbv=Super Fast,DegreePlanName=As Fast as I can,FK:DegreeID=1},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1">
       <c r="A7" s="9">
         <v>7254</v>
       </c>
@@ -5879,13 +5594,17 @@
         <v>533623</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" s="9">
         <v>1</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f>"DegreePlan {"&amp;$A$1&amp;"="&amp;A7&amp;", "&amp;$B$1&amp;"="&amp;B7&amp;", "&amp;$C$1&amp;"="&amp;C7&amp;","&amp;$D$1&amp;"="&amp;D7&amp;","&amp;$E$1&amp;"="&amp;E7&amp;"},"</f>
+        <v>DegreePlan {DegreePlanID=7254, StudentID=533623, DegreePlanAbv=Slow and Easy,DegreePlanName=As slow as I can,FK:DegreeID=1},</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -6876,10 +6595,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E999"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6891,24 +6610,27 @@
     <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -6919,13 +6641,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1">
+        <v>72</v>
+      </c>
+      <c r="F2" s="8">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -6936,13 +6661,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1">
+        <v>74</v>
+      </c>
+      <c r="F3" s="8">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -6953,13 +6681,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1">
+        <v>76</v>
+      </c>
+      <c r="F4" s="8">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -6970,13 +6701,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1">
+        <v>78</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -6987,13 +6721,16 @@
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1">
+        <v>80</v>
+      </c>
+      <c r="F6" s="8">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -7004,13 +6741,16 @@
         <v>6</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1">
+        <v>82</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="5" customFormat="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -7021,13 +6761,16 @@
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1">
+        <v>82</v>
+      </c>
+      <c r="F8" s="5">
+        <v>7255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -7038,13 +6781,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1">
+        <v>84</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -7055,13 +6801,16 @@
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1">
+        <v>86</v>
+      </c>
+      <c r="F10" s="5">
+        <v>7255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -7072,13 +6821,16 @@
         <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1">
+        <v>88</v>
+      </c>
+      <c r="F11" s="5">
+        <v>7255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="5" customFormat="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -7089,13 +6841,16 @@
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="7" customFormat="1">
+        <v>90</v>
+      </c>
+      <c r="F12" s="5">
+        <v>7255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="7" customFormat="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -7106,13 +6861,16 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="7" customFormat="1">
+        <v>91</v>
+      </c>
+      <c r="F13" s="7">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="7" customFormat="1">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -7123,13 +6881,16 @@
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="7" customFormat="1">
+        <v>92</v>
+      </c>
+      <c r="F14" s="7">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="7" customFormat="1">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -7140,13 +6901,16 @@
         <v>3</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="7" customFormat="1">
+        <v>94</v>
+      </c>
+      <c r="F15" s="7">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="7" customFormat="1">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -7157,13 +6921,16 @@
         <v>4</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="7" customFormat="1">
+        <v>95</v>
+      </c>
+      <c r="F16" s="7">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="7" customFormat="1">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -7174,37 +6941,40 @@
         <v>5</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>96</v>
+      </c>
+      <c r="F17" s="7">
+        <v>7254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -8180,10 +7950,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E998"/>
+  <dimension ref="A1:E933"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8197,1348 +7967,308 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1">
-      <c r="A2" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="B2" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
+        <v>356</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>542</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>563</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
         <v>460</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1">
-      <c r="A3" s="8">
+      <c r="E5" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C6" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>542</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1">
-      <c r="A4" s="8">
+      <c r="D6" s="7">
+        <v>560</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>664</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>64</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C9" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>563</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1">
-      <c r="A5" s="8">
+      <c r="D9" s="10">
+        <v>618</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>691</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C11" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C5" s="8">
-        <v>2</v>
-      </c>
-      <c r="D5" s="8">
-        <v>356</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1">
-      <c r="A6" s="8">
+      <c r="D11" s="10">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4</v>
+      </c>
+      <c r="D12" s="10">
+        <v>555</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C13" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C6" s="8">
-        <v>2</v>
-      </c>
-      <c r="D6" s="8">
-        <v>643</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8">
-        <v>664</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C8" s="8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8">
-        <v>560</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C9" s="8">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8">
-        <v>618</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1">
-      <c r="A10" s="8">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C10" s="8">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8">
-        <v>691</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1">
-      <c r="A11" s="8">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C11" s="8">
-        <v>4</v>
-      </c>
-      <c r="D11" s="8">
-        <v>555</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C12" s="8">
-        <v>4</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="D13" s="10">
+        <v>20</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>7255</v>
+      </c>
+      <c r="C14" s="7">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10">
         <v>692</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1">
-      <c r="A13" s="8">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C13" s="8">
-        <v>4</v>
-      </c>
-      <c r="D13" s="8">
-        <v>10</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="8" customFormat="1">
-      <c r="A14" s="8">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8">
-        <v>7251</v>
-      </c>
-      <c r="C14" s="8">
-        <v>4</v>
-      </c>
-      <c r="D14" s="8">
-        <v>20</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="5">
-        <v>460</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5">
-        <v>356</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <v>542</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="5" customFormat="1">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5">
-        <v>563</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C19" s="5">
-        <v>2</v>
-      </c>
-      <c r="D19" s="9">
-        <v>560</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="5" customFormat="1">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C20" s="5">
-        <v>2</v>
-      </c>
-      <c r="D20" s="9">
-        <v>618</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C21" s="5">
-        <v>3</v>
-      </c>
-      <c r="D21" s="9">
-        <v>664</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C22" s="5">
-        <v>3</v>
-      </c>
-      <c r="D22" s="9">
-        <v>555</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C23" s="5">
-        <v>3</v>
-      </c>
-      <c r="D23" s="9">
-        <v>691</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C24" s="5">
-        <v>3</v>
-      </c>
-      <c r="D24" s="9">
-        <v>10</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C25" s="5">
-        <v>4</v>
-      </c>
-      <c r="D25" s="9">
-        <v>692</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C26" s="5">
-        <v>4</v>
-      </c>
-      <c r="D26" s="9">
-        <v>643</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5">
-        <v>7253</v>
-      </c>
-      <c r="C27" s="5">
-        <v>4</v>
-      </c>
-      <c r="D27" s="9">
-        <v>20</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A28" s="7">
-        <v>27</v>
-      </c>
-      <c r="B28" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C28" s="7">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7">
-        <v>356</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="7">
-        <v>28</v>
-      </c>
-      <c r="B29" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C29" s="7">
-        <v>1</v>
-      </c>
-      <c r="D29" s="7">
-        <v>542</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="7">
-        <v>29</v>
-      </c>
-      <c r="B30" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C30" s="7">
-        <v>1</v>
-      </c>
-      <c r="D30" s="7">
-        <v>563</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="7">
-        <v>30</v>
-      </c>
-      <c r="B31" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7">
-        <v>460</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="7">
-        <v>31</v>
-      </c>
-      <c r="B32" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C32" s="7">
-        <v>2</v>
-      </c>
-      <c r="D32" s="7">
-        <v>560</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="7">
-        <v>32</v>
-      </c>
-      <c r="B33" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C33" s="7">
-        <v>2</v>
-      </c>
-      <c r="D33" s="7">
-        <v>664</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="7">
-        <v>33</v>
-      </c>
-      <c r="B34" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C34" s="7">
-        <v>2</v>
-      </c>
-      <c r="D34" s="7">
-        <v>64</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="7">
-        <v>34</v>
-      </c>
-      <c r="B35" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C35" s="7">
-        <v>3</v>
-      </c>
-      <c r="D35" s="10">
-        <v>618</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="7">
-        <v>35</v>
-      </c>
-      <c r="B36" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C36" s="7">
-        <v>3</v>
-      </c>
-      <c r="D36" s="10">
-        <v>691</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="7">
-        <v>36</v>
-      </c>
-      <c r="B37" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C37" s="7">
-        <v>4</v>
-      </c>
-      <c r="D37" s="10">
-        <v>10</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="7">
-        <v>37</v>
-      </c>
-      <c r="B38" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C38" s="7">
-        <v>4</v>
-      </c>
-      <c r="D38" s="10">
-        <v>555</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A39" s="7">
-        <v>38</v>
-      </c>
-      <c r="B39" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C39" s="7">
-        <v>5</v>
-      </c>
-      <c r="D39" s="10">
-        <v>20</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A40" s="7">
-        <v>39</v>
-      </c>
-      <c r="B40" s="10">
-        <v>7255</v>
-      </c>
-      <c r="C40" s="7">
-        <v>5</v>
-      </c>
-      <c r="D40" s="10">
-        <v>692</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A41" s="7">
-        <v>40</v>
-      </c>
-      <c r="B41" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C41" s="7">
-        <v>1</v>
-      </c>
-      <c r="D41" s="7">
-        <v>460</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A42" s="7">
-        <v>41</v>
-      </c>
-      <c r="B42" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C42" s="7">
-        <v>1</v>
-      </c>
-      <c r="D42" s="7">
-        <v>356</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A43" s="7">
-        <v>42</v>
-      </c>
-      <c r="B43" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C43" s="7">
-        <v>1</v>
-      </c>
-      <c r="D43" s="7">
-        <v>542</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A44" s="7">
-        <v>43</v>
-      </c>
-      <c r="B44" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C44" s="7">
-        <v>1</v>
-      </c>
-      <c r="D44" s="7">
-        <v>563</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A45" s="7">
-        <v>44</v>
-      </c>
-      <c r="B45" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C45" s="7">
-        <v>2</v>
-      </c>
-      <c r="D45" s="7">
-        <v>560</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A46" s="7">
-        <v>45</v>
-      </c>
-      <c r="B46" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C46" s="7">
-        <v>2</v>
-      </c>
-      <c r="D46" s="7">
-        <v>64</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A47" s="7">
-        <v>46</v>
-      </c>
-      <c r="B47" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C47" s="7">
-        <v>2</v>
-      </c>
-      <c r="D47" s="7">
-        <v>555</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A48" s="7">
-        <v>47</v>
-      </c>
-      <c r="B48" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C48" s="7">
-        <v>3</v>
-      </c>
-      <c r="D48" s="7">
-        <v>618</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A49" s="7">
-        <v>48</v>
-      </c>
-      <c r="B49" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C49" s="7">
-        <v>3</v>
-      </c>
-      <c r="D49" s="7">
-        <v>691</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="7">
-        <v>49</v>
-      </c>
-      <c r="B50" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C50" s="7">
-        <v>4</v>
-      </c>
-      <c r="D50" s="7">
-        <v>10</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A51" s="7">
-        <v>50</v>
-      </c>
-      <c r="B51" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C51" s="7">
-        <v>4</v>
-      </c>
-      <c r="D51" s="7">
-        <v>20</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A52" s="7">
-        <v>51</v>
-      </c>
-      <c r="B52" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C52" s="7">
-        <v>4</v>
-      </c>
-      <c r="D52" s="7">
-        <v>664</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A53" s="7">
-        <v>52</v>
-      </c>
-      <c r="B53" s="7">
-        <v>7257</v>
-      </c>
-      <c r="C53" s="7">
-        <v>4</v>
-      </c>
-      <c r="D53" s="7">
-        <v>692</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A54" s="8">
+      <c r="E14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C54" s="8">
-        <v>1</v>
-      </c>
-      <c r="D54" s="8">
-        <v>460</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A55" s="8">
-        <v>54</v>
-      </c>
-      <c r="B55" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C55" s="8">
-        <v>1</v>
-      </c>
-      <c r="D55" s="8">
-        <v>356</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A56" s="8">
-        <v>55</v>
-      </c>
-      <c r="B56" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C56" s="8">
-        <v>1</v>
-      </c>
-      <c r="D56" s="8">
-        <v>542</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A57" s="8">
-        <v>56</v>
-      </c>
-      <c r="B57" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C57" s="8">
-        <v>1</v>
-      </c>
-      <c r="D57" s="8">
-        <v>563</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A58" s="8">
-        <v>59</v>
-      </c>
-      <c r="B58" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C58" s="8">
-        <v>2</v>
-      </c>
-      <c r="D58" s="8">
-        <v>691</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A59" s="8">
-        <v>60</v>
-      </c>
-      <c r="B59" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C59" s="8">
-        <v>2</v>
-      </c>
-      <c r="D59" s="8">
-        <v>618</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A60" s="8">
-        <v>61</v>
-      </c>
-      <c r="B60" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C60" s="8">
-        <v>3</v>
-      </c>
-      <c r="D60" s="8">
-        <v>692</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A61" s="8">
-        <v>62</v>
-      </c>
-      <c r="B61" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C61" s="8">
-        <v>3</v>
-      </c>
-      <c r="D61" s="8">
-        <v>560</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A62" s="8">
-        <v>63</v>
-      </c>
-      <c r="B62" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C62" s="8">
-        <v>4</v>
-      </c>
-      <c r="D62" s="8">
-        <v>555</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="8">
-        <v>64</v>
-      </c>
-      <c r="B63" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C63" s="8">
-        <v>4</v>
-      </c>
-      <c r="D63" s="8">
-        <v>643</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A64" s="8">
-        <v>65</v>
-      </c>
-      <c r="B64" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C64" s="8">
-        <v>4</v>
-      </c>
-      <c r="D64" s="8">
-        <v>20</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A65" s="8">
-        <v>66</v>
-      </c>
-      <c r="B65" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C65" s="8">
-        <v>6</v>
-      </c>
-      <c r="D65" s="8">
-        <v>10</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A66" s="8">
-        <v>67</v>
-      </c>
-      <c r="B66" s="8">
-        <v>7258</v>
-      </c>
-      <c r="C66" s="8">
-        <v>6</v>
-      </c>
-      <c r="D66" s="8">
-        <v>664</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A67" s="5">
-        <v>68</v>
-      </c>
-      <c r="B67" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C67" s="9">
-        <v>1</v>
-      </c>
-      <c r="D67" s="9">
-        <v>460</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A68" s="5">
-        <v>69</v>
-      </c>
-      <c r="B68" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C68" s="9">
-        <v>1</v>
-      </c>
-      <c r="D68" s="9">
-        <v>356</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A69" s="5">
-        <v>70</v>
-      </c>
-      <c r="B69" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C69" s="9">
-        <v>1</v>
-      </c>
-      <c r="D69" s="9">
-        <v>542</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A70" s="5">
-        <v>71</v>
-      </c>
-      <c r="B70" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C70" s="9">
-        <v>2</v>
-      </c>
-      <c r="D70" s="9">
-        <v>560</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A71" s="5">
-        <v>72</v>
-      </c>
-      <c r="B71" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C71" s="9">
-        <v>2</v>
-      </c>
-      <c r="D71" s="9">
-        <v>664</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A72" s="5">
-        <v>73</v>
-      </c>
-      <c r="B72" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C72" s="9">
-        <v>2</v>
-      </c>
-      <c r="D72" s="9">
-        <v>10</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A73" s="5">
-        <v>74</v>
-      </c>
-      <c r="B73" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C73" s="9">
-        <v>3</v>
-      </c>
-      <c r="D73" s="9">
-        <v>618</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A74" s="5">
-        <v>75</v>
-      </c>
-      <c r="B74" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C74" s="9">
-        <v>3</v>
-      </c>
-      <c r="D74" s="9">
-        <v>691</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="5">
-        <v>76</v>
-      </c>
-      <c r="B75" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C75" s="9">
-        <v>4</v>
-      </c>
-      <c r="D75" s="9">
-        <v>692</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A76" s="5">
-        <v>77</v>
-      </c>
-      <c r="B76" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C76" s="9">
-        <v>4</v>
-      </c>
-      <c r="D76" s="9">
-        <v>20</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A77" s="5">
-        <v>78</v>
-      </c>
-      <c r="B77" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C77" s="9">
-        <v>4</v>
-      </c>
-      <c r="D77" s="9">
-        <v>555</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A78" s="5">
-        <v>79</v>
-      </c>
-      <c r="B78" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C78" s="9">
-        <v>5</v>
-      </c>
-      <c r="D78" s="9">
-        <v>563</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="5" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A79" s="5">
-        <v>80</v>
-      </c>
-      <c r="B79" s="9">
-        <v>7254</v>
-      </c>
-      <c r="C79" s="9">
-        <v>5</v>
-      </c>
-      <c r="D79" s="9">
-        <v>64</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -10392,71 +9122,6 @@
     <row r="931" ht="15.75" customHeight="1"/>
     <row r="932" ht="15.75" customHeight="1"/>
     <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
committing foreign key references
</commit_message>
<xml_diff>
--- a/dotnet.xlsx
+++ b/dotnet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533623\Documents\44663\Degreeplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533619\Documents\44663\Degreeplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="4545" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="4545" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
   <si>
     <t>PK: DegreeID</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>FK:StudentID</t>
   </si>
   <si>
     <t>Term</t>
@@ -764,7 +761,7 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1">
@@ -1847,7 +1844,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1865,7 +1862,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1876,7 +1873,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1972,7 +1969,7 @@
         <v>560</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3186,16 +3183,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1">
@@ -4435,22 +4432,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
         <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1">
@@ -5522,10 +5519,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
@@ -5534,10 +5531,10 @@
         <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1">
@@ -6654,28 +6651,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G999"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" customWidth="1"/>
-    <col min="8" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="102.42578125" customWidth="1"/>
+    <col min="7" max="25" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
       </c>
       <c r="C1" t="s">
@@ -6685,424 +6681,373 @@
         <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="8">
-        <v>533619</v>
-      </c>
-      <c r="C2" s="8">
         <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="E2" s="8">
         <v>7258</v>
       </c>
-      <c r="G2" s="8" t="str">
-        <f xml:space="preserve"> "new StudentTerm{"&amp;$A$1&amp;" = "&amp;A2 &amp;" , "&amp;$B$1 &amp;" = "&amp;B2&amp;" , "&amp;$C$1 &amp;" = "&amp;C2 &amp;" , "&amp;$D$1 &amp;" = "&amp;D2 &amp;" , "&amp;$E$1&amp;" = "&amp;E2 &amp;" , "&amp;$F$1&amp;"="&amp;F2&amp;"},"</f>
-        <v>new StudentTerm{ StudentTermID = 1 , FK:StudentID = 533619 , Term = 1 , TermAbv = S18 , TermName = Spring 2018 , DegreeplanID=7258},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1">
+      <c r="F2" s="8" t="str">
+        <f xml:space="preserve"> "new StudentTerm{"&amp;$A$1&amp;" = "&amp;A2 &amp;" , "&amp;$B$1 &amp;" = "&amp;B2&amp;" , "&amp;$C$1 &amp;" = "&amp;C2 &amp;" , "&amp;$D$1 &amp;" = "&amp;D2 &amp;" , "&amp;$E$1&amp;" = "&amp;E2 &amp;"},"</f>
+        <v>new StudentTerm{ StudentTermID = 1 , Term = 1 , TermAbv = S18 , TermName = Spring 2018 , DegreeplanID = 7258},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="8">
-        <v>533619</v>
-      </c>
-      <c r="C3" s="8">
         <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="8">
         <v>7258</v>
       </c>
-      <c r="G3" s="8" t="str">
-        <f t="shared" ref="G3:G17" si="0" xml:space="preserve"> "new StudentTerm{"&amp;$A$1&amp;" = "&amp;A3 &amp;" , "&amp;$B$1 &amp;" = "&amp;B3&amp;" , "&amp;$C$1 &amp;" = "&amp;C3 &amp;" , "&amp;$D$1 &amp;" = "&amp;D3 &amp;" , "&amp;$E$1&amp;" = "&amp;E3 &amp;" , "&amp;$F$1&amp;" ="&amp;F3&amp;"},"</f>
-        <v>new StudentTerm{ StudentTermID = 2 , FK:StudentID = 533619 , Term = 2 , TermAbv = Su18 , TermName = Summer 2018 , DegreeplanID =7258},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1">
+      <c r="F3" s="8" t="str">
+        <f t="shared" ref="F3:F17" si="0" xml:space="preserve"> "new StudentTerm{"&amp;$A$1&amp;" = "&amp;A3 &amp;" , "&amp;$B$1 &amp;" = "&amp;B3&amp;" , "&amp;$C$1 &amp;" = "&amp;C3 &amp;" , "&amp;$D$1 &amp;" = "&amp;D3 &amp;" , "&amp;$E$1&amp;" = "&amp;E3 &amp;"},"</f>
+        <v>new StudentTerm{ StudentTermID = 2 , Term = 2 , TermAbv = Su18 , TermName = Summer 2018 , DegreeplanID = 7258},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="8">
-        <v>533619</v>
-      </c>
-      <c r="C4" s="8">
         <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="8">
         <v>7258</v>
       </c>
-      <c r="G4" s="8" t="str">
+      <c r="F4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 3 , FK:StudentID = 533619 , Term = 3 , TermAbv = F18 , TermName = Fall 2018 , DegreeplanID =7258},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="8" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 3 , Term = 3 , TermAbv = F18 , TermName = Fall 2018 , DegreeplanID = 7258},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="8">
-        <v>533619</v>
-      </c>
-      <c r="C5" s="8">
         <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="8">
         <v>7258</v>
       </c>
-      <c r="G5" s="8" t="str">
+      <c r="F5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 4 , FK:StudentID = 533619 , Term = 4 , TermAbv = S19 , TermName = Spring 2019 , DegreeplanID =7258},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="8" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 4 , Term = 4 , TermAbv = S19 , TermName = Spring 2019 , DegreeplanID = 7258},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="8">
-        <v>533619</v>
-      </c>
-      <c r="C6" s="8">
         <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="E6" s="8">
         <v>7258</v>
       </c>
-      <c r="G6" s="8" t="str">
+      <c r="F6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 5 , FK:StudentID = 533619 , Term = 5 , TermAbv = Su19 , TermName = Summer 2019 , DegreeplanID =7258},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="8" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 5 , Term = 5 , TermAbv = Su19 , TermName = Summer 2019 , DegreeplanID = 7258},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="8">
-        <v>533619</v>
-      </c>
-      <c r="C7" s="8">
         <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="8">
         <v>7258</v>
       </c>
-      <c r="G7" s="8" t="str">
+      <c r="F7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 6 , FK:StudentID = 533619 , Term = 6 , TermAbv = F19 , TermName = Fall 2019 , DegreeplanID =7258},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 6 , Term = 6 , TermAbv = F19 , TermName = Fall 2019 , DegreeplanID = 7258},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="5" customFormat="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>533623</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="B8" s="9">
         <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="E8" s="5">
         <v>7255</v>
       </c>
-      <c r="G8" s="8" t="str">
+      <c r="F8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 7 , FK:StudentID = 533623 , Term = 1 , TermAbv = F19 , TermName = Fall 2019 , DegreeplanID =7255},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 7 , Term = 1 , TermAbv = F19 , TermName = Fall 2019 , DegreeplanID = 7255},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
-        <v>533623</v>
-      </c>
-      <c r="C9" s="9">
+      <c r="B9" s="9">
         <v>2</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9" s="5">
         <v>7255</v>
       </c>
-      <c r="G9" s="8" t="str">
+      <c r="F9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 8 , FK:StudentID = 533623 , Term = 2 , TermAbv = S20 , TermName = Spring 2020 , DegreeplanID =7255},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 8 , Term = 2 , TermAbv = S20 , TermName = Spring 2020 , DegreeplanID = 7255},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
-        <v>533623</v>
-      </c>
-      <c r="C10" s="9">
+      <c r="B10" s="9">
         <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="E10" s="5">
         <v>7255</v>
       </c>
-      <c r="G10" s="8" t="str">
+      <c r="F10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 9 , FK:StudentID = 533623 , Term = 3 , TermAbv = Su20 , TermName = Summer 2020 , DegreeplanID =7255},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="5" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 9 , Term = 3 , TermAbv = Su20 , TermName = Summer 2020 , DegreeplanID = 7255},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
-        <v>533623</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="B11" s="9">
         <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E11" s="5">
         <v>7255</v>
       </c>
-      <c r="G11" s="8" t="str">
+      <c r="F11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 10 , FK:StudentID = 533623 , Term = 4 , TermAbv = F20 , TermName = Fall 2020 , DegreeplanID =7255},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 10 , Term = 4 , TermAbv = F20 , TermName = Fall 2020 , DegreeplanID = 7255},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="5" customFormat="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
-        <v>533623</v>
-      </c>
-      <c r="C12" s="9">
+      <c r="B12" s="9">
         <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="E12" s="5">
         <v>7255</v>
       </c>
-      <c r="G12" s="8" t="str">
+      <c r="F12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 11 , FK:StudentID = 533623 , Term = 5 , TermAbv = S21 , TermName = Spring 2021 , DegreeplanID =7255},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 11 , Term = 5 , TermAbv = S21 , TermName = Spring 2021 , DegreeplanID = 7255},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="7" customFormat="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="7">
-        <v>533907</v>
-      </c>
-      <c r="C13" s="7">
         <v>1</v>
       </c>
+      <c r="C13" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="D13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="7">
+        <v>82</v>
+      </c>
+      <c r="E13" s="7">
         <v>7254</v>
       </c>
-      <c r="G13" s="8" t="str">
+      <c r="F13" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 12 , FK:StudentID = 533907 , Term = 1 , TermAbv = F18 , TermName = Fall2018 , DegreeplanID =7254},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="7" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 12 , Term = 1 , TermAbv = F18 , TermName = Fall2018 , DegreeplanID = 7254},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="7" customFormat="1">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="7">
-        <v>533907</v>
-      </c>
-      <c r="C14" s="7">
         <v>2</v>
       </c>
+      <c r="C14" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="7">
+        <v>83</v>
+      </c>
+      <c r="E14" s="7">
         <v>7254</v>
       </c>
-      <c r="G14" s="8" t="str">
+      <c r="F14" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 13 , FK:StudentID = 533907 , Term = 2 , TermAbv = S19 , TermName = Spring2019 , DegreeplanID =7254},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="7" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 13 , Term = 2 , TermAbv = S19 , TermName = Spring2019 , DegreeplanID = 7254},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="7" customFormat="1">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="7">
-        <v>533907</v>
-      </c>
-      <c r="C15" s="7">
         <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="E15" s="7">
         <v>7254</v>
       </c>
-      <c r="G15" s="8" t="str">
+      <c r="F15" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 14 , FK:StudentID = 533907 , Term = 3 , TermAbv = SU19 , TermName = Summer2019 , DegreeplanID =7254},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="7" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 14 , Term = 3 , TermAbv = SU19 , TermName = Summer2019 , DegreeplanID = 7254},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="7" customFormat="1">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="7">
-        <v>533907</v>
-      </c>
-      <c r="C16" s="7">
         <v>4</v>
       </c>
+      <c r="C16" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="D16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="7">
+        <v>86</v>
+      </c>
+      <c r="E16" s="7">
         <v>7254</v>
       </c>
-      <c r="G16" s="8" t="str">
+      <c r="F16" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 15 , FK:StudentID = 533907 , Term = 4 , TermAbv = F20 , TermName = Fall2019 , DegreeplanID =7254},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="7" customFormat="1">
+        <v>new StudentTerm{ StudentTermID = 15 , Term = 4 , TermAbv = F20 , TermName = Fall2019 , DegreeplanID = 7254},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="7" customFormat="1">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="7">
-        <v>533907</v>
-      </c>
-      <c r="C17" s="7">
         <v>5</v>
       </c>
+      <c r="C17" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="D17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="7">
+        <v>87</v>
+      </c>
+      <c r="E17" s="7">
         <v>7254</v>
       </c>
-      <c r="G17" s="8" t="str">
+      <c r="F17" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{ StudentTermID = 16 , FK:StudentID = 533907 , Term = 5 , TermAbv = S20 , TermName = Spring2020 , DegreeplanID =7254},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>new StudentTerm{ StudentTermID = 16 , Term = 5 , TermAbv = S20 , TermName = Spring2020 , DegreeplanID = 7254},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:6">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -8080,7 +8025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F933"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -8095,22 +8040,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
         <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">

</xml_diff>